<commit_message>
currently functioning spacy determiner
</commit_message>
<xml_diff>
--- a/training_spacy/entity_data.xlsx
+++ b/training_spacy/entity_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriaarmstrong/Desktop/contingent-plan-executor/training_spacy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC371391-9C2C-B24F-9F2D-6BD2403FA472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DC4B4F-F3F3-4246-8BEB-83AB7E4455C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16440" xr2:uid="{0035BE3F-1E58-874C-B2FD-8BA3574D7306}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25780" windowHeight="16440" xr2:uid="{0035BE3F-1E58-874C-B2FD-8BA3574D7306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>utterance</t>
   </si>
@@ -206,20 +206,38 @@
     <t>low, high</t>
   </si>
   <si>
-    <t>fun, exciting, social, chill, relaxing, laid-back</t>
-  </si>
-  <si>
-    <t>(low fun),(low exciting),(low social),(low chill),(low relaxing),(low laid-back),(high fun),(high exciting),(high social),(high chill),(high relaxing),(high laid-back)</t>
-  </si>
-  <si>
     <t>BUDGET,OUTING_TYPE</t>
+  </si>
+  <si>
+    <t>(low fun),(low exciting),(low social),(low chill),(low relaxing),(low laid-back), (low low-energy), (low high-energy), (high fun),(high exciting),(high social),(high chill),(high relaxing),(high laid-back), (high low-energy), (high high-energy)</t>
+  </si>
+  <si>
+    <t>fun, exciting, social, chill, relaxing, laid-back, low-energy, high-energy</t>
+  </si>
+  <si>
+    <t>"My address is 123 Westwind."</t>
+  </si>
+  <si>
+    <t>"My phone number is $."</t>
+  </si>
+  <si>
+    <t>"My number is $."</t>
+  </si>
+  <si>
+    <t>"$"</t>
+  </si>
+  <si>
+    <t>6133992081, 2137584930, 2637490563, 2635478152, 613 399 2081, 213 758 4930, 263 749 0563, 263 547 8152, 613-399-2081, 213-758-4930, 263-749-0563, 263-547-8152</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +256,13 @@
       <color rgb="FF6AAB73"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,9 +285,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE64575-9834-AC4F-8CE4-DF19021BC1B3}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -816,7 +842,7 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -827,7 +853,7 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -838,7 +864,7 @@
         <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -879,45 +905,110 @@
         <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>